<commit_message>
add function combine geojson
</commit_message>
<xml_diff>
--- a/public/data/DATA DATA/Jumlah Penduduk miskin 2010-2019.xlsx
+++ b/public/data/DATA DATA/Jumlah Penduduk miskin 2010-2019.xlsx
@@ -1,33 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WORK\2020\PIM 4\AP\BAHAN ANALISIS\DATA DATA\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView windowWidth="20490" windowHeight="7830" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ABDYA 2010-2019" sheetId="3" r:id="rId1"/>
     <sheet name="Aceh" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
+    <t>Jumlah Penduduk Miskin Kabupaten Aceh Barat Daya Tahun 2010-2019 (ribuan)</t>
+  </si>
+  <si>
+    <t>Kabupaten/Kota</t>
+  </si>
+  <si>
+    <t>Tahun</t>
+  </si>
+  <si>
+    <t>Aceh Barat Daya</t>
+  </si>
+  <si>
+    <t>Jumlah Penduduk Miskin Menurut Kabupaten/Kota di Provinsi Aceh Tahun 2010-2019 (ribuan)</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>Simeulue</t>
   </si>
   <si>
@@ -61,9 +69,6 @@
     <t>Aceh Utara</t>
   </si>
   <si>
-    <t>Aceh Barat Daya</t>
-  </si>
-  <si>
     <t>Gayo Lues</t>
   </si>
   <si>
@@ -98,47 +103,25 @@
   </si>
   <si>
     <t>Aceh</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Kabupaten/Kota</t>
-  </si>
-  <si>
-    <t>Tahun</t>
-  </si>
-  <si>
-    <t>Jumlah Penduduk Miskin Menurut Kabupaten/Kota di Provinsi Aceh Tahun 2010-2019 (ribuan)</t>
-  </si>
-  <si>
-    <t>Jumlah Penduduk Miskin Kabupaten Aceh Barat Daya Tahun 2010-2019 (ribuan)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;_-;_-@_-"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="6">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
@@ -146,17 +129,168 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,8 +303,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -180,110 +500,388 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -332,7 +930,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -367,7 +965,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -541,244 +1139,241 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="B1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="12" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.14285714285714" style="1"/>
+    <col min="2" max="2" width="18.4285714285714" style="1" customWidth="1"/>
+    <col min="3" max="12" width="9.85714285714286" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B1" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-    </row>
-    <row r="3" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+    <row r="1" spans="2:13">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="3" ht="15" customHeight="1" spans="2:12">
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" ht="15" spans="2:12">
+      <c r="B4" s="3"/>
+      <c r="C4" s="4">
+        <v>2010</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2011</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2012</v>
+      </c>
+      <c r="F4" s="4">
+        <v>2013</v>
+      </c>
+      <c r="G4" s="4">
+        <v>2014</v>
+      </c>
+      <c r="H4" s="4">
+        <v>2015</v>
+      </c>
+      <c r="I4" s="4">
+        <v>2016</v>
+      </c>
+      <c r="J4" s="4">
+        <v>2017</v>
+      </c>
+      <c r="K4" s="4">
+        <v>2018</v>
+      </c>
+      <c r="L4" s="4">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="15">
+        <v>25.2</v>
+      </c>
+      <c r="D5" s="15">
+        <v>25.2530201491707</v>
+      </c>
+      <c r="E5" s="15">
+        <v>24.63545</v>
+      </c>
+      <c r="F5" s="15">
+        <v>25.7</v>
+      </c>
+      <c r="G5" s="15">
         <v>25</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-    </row>
-    <row r="4" spans="2:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="B4" s="11"/>
-      <c r="C4" s="2">
-        <v>2010</v>
-      </c>
-      <c r="D4" s="2">
-        <v>2011</v>
-      </c>
-      <c r="E4" s="2">
-        <v>2012</v>
-      </c>
-      <c r="F4" s="2">
-        <v>2013</v>
-      </c>
-      <c r="G4" s="2">
-        <v>2014</v>
-      </c>
-      <c r="H4" s="2">
-        <v>2015</v>
-      </c>
-      <c r="I4" s="2">
-        <v>2016</v>
-      </c>
-      <c r="J4" s="2">
-        <v>2017</v>
-      </c>
-      <c r="K4" s="2">
-        <v>2018</v>
-      </c>
-      <c r="L4" s="2">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="10">
-        <v>25.2</v>
-      </c>
-      <c r="D5" s="10">
-        <v>25.253020149170659</v>
-      </c>
-      <c r="E5" s="10">
-        <v>24.635449999999999</v>
-      </c>
-      <c r="F5" s="10">
-        <v>25.7</v>
-      </c>
-      <c r="G5" s="10">
-        <v>25</v>
-      </c>
-      <c r="H5" s="10">
+      <c r="H5" s="15">
         <v>25.93</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="15">
         <v>25.73</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="15">
         <v>26.573</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="15">
         <v>25.23</v>
       </c>
-      <c r="L5" s="10">
-        <v>24.364000000000001</v>
+      <c r="L5" s="15">
+        <v>24.364</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="C3:L3"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:L3"/>
-    <mergeCell ref="B1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="B1:M28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:M16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.14285714285714" style="1"/>
+    <col min="2" max="2" width="3.57142857142857" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.4285714285714" style="1" customWidth="1"/>
+    <col min="4" max="13" width="9.85714285714286" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B1" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-    </row>
-    <row r="3" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-    </row>
-    <row r="4" spans="2:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="2">
+    <row r="1" spans="2:13">
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="3" ht="15" customHeight="1" spans="2:13">
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" ht="15" spans="2:13">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4">
         <v>2010</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="4">
         <v>2011</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="4">
         <v>2012</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="4">
         <v>2013</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="4">
         <v>2014</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="4">
         <v>2015</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="4">
         <v>2016</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="4">
         <v>2017</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="4">
         <v>2018</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="4">
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B5" s="4">
+    <row r="5" spans="2:13">
+      <c r="B5" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>0</v>
+      <c r="C5" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="D5" s="7">
-        <v>18.899999999999999</v>
+        <v>18.9</v>
       </c>
       <c r="E5" s="7">
-        <v>19.039975509295338</v>
+        <v>19.0399755092953</v>
       </c>
       <c r="F5" s="7">
-        <v>18.501429999999999</v>
+        <v>18.50143</v>
       </c>
       <c r="G5" s="7">
         <v>17.8</v>
@@ -799,24 +1394,24 @@
         <v>18.22</v>
       </c>
       <c r="M5" s="7">
-        <v>17.667000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B6" s="4">
+        <v>17.667</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13">
+      <c r="B6" s="5">
         <v>2</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>1</v>
+      <c r="C6" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="D6" s="7">
-        <v>19.899999999999999</v>
+        <v>19.9</v>
       </c>
       <c r="E6" s="7">
-        <v>19.94186908605143</v>
+        <v>19.9418690860514</v>
       </c>
       <c r="F6" s="7">
-        <v>19.377479999999998</v>
+        <v>19.37748</v>
       </c>
       <c r="G6" s="7">
         <v>20.7</v>
@@ -831,27 +1426,27 @@
         <v>25.09</v>
       </c>
       <c r="K6" s="7">
-        <v>26.265999999999998</v>
+        <v>26.266</v>
       </c>
       <c r="L6" s="7">
         <v>25.74</v>
       </c>
       <c r="M6" s="7">
-        <v>25.661000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="4">
+        <v>25.661</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13">
+      <c r="B7" s="5">
         <v>3</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>2</v>
+      <c r="C7" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="D7" s="7">
-        <v>32.200000000000003</v>
+        <v>32.2</v>
       </c>
       <c r="E7" s="7">
-        <v>32.267747968384725</v>
+        <v>32.2677479683847</v>
       </c>
       <c r="F7" s="7">
         <v>31.4513</v>
@@ -878,21 +1473,21 @@
         <v>31.06</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="4">
+    <row r="8" spans="2:13">
+      <c r="B8" s="5">
         <v>4</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>3</v>
+      <c r="C8" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="D8" s="7">
         <v>30</v>
       </c>
       <c r="E8" s="7">
-        <v>30.163329622620505</v>
+        <v>30.1633296226205</v>
       </c>
       <c r="F8" s="7">
-        <v>29.406759999999998</v>
+        <v>29.40676</v>
       </c>
       <c r="G8" s="7">
         <v>27.8</v>
@@ -907,33 +1502,33 @@
         <v>29.39</v>
       </c>
       <c r="K8" s="7">
-        <v>30.835000000000001</v>
+        <v>30.835</v>
       </c>
       <c r="L8" s="7">
         <v>30.2</v>
       </c>
       <c r="M8" s="7">
-        <v>28.928999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B9" s="4">
+        <v>28.929</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13">
+      <c r="B9" s="5">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>4</v>
+      <c r="C9" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="D9" s="7">
         <v>66.5</v>
       </c>
       <c r="E9" s="7">
-        <v>66.740124679951052</v>
+        <v>66.7401246799511</v>
       </c>
       <c r="F9" s="7">
-        <v>64.948849999999993</v>
+        <v>64.94885</v>
       </c>
       <c r="G9" s="7">
-        <v>64.400000000000006</v>
+        <v>64.4</v>
       </c>
       <c r="H9" s="7">
         <v>63</v>
@@ -945,68 +1540,68 @@
         <v>61.63</v>
       </c>
       <c r="K9" s="7">
-        <v>63.670999999999999</v>
+        <v>63.671</v>
       </c>
       <c r="L9" s="7">
         <v>61.64</v>
       </c>
       <c r="M9" s="7">
-        <v>62.792999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="4">
+        <v>62.793</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13">
+      <c r="B10" s="5">
         <v>6</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>5</v>
+      <c r="C10" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="D10" s="7">
-        <v>35.299999999999997</v>
+        <v>35.3</v>
       </c>
       <c r="E10" s="7">
-        <v>35.374270288322393</v>
+        <v>35.3742702883224</v>
       </c>
       <c r="F10" s="7">
-        <v>34.469819999999999</v>
+        <v>34.46982</v>
       </c>
       <c r="G10" s="7">
         <v>33.6</v>
       </c>
       <c r="H10" s="7">
-        <v>32.799999999999997</v>
+        <v>32.8</v>
       </c>
       <c r="I10" s="7">
         <v>34.26</v>
       </c>
       <c r="J10" s="7">
-        <v>33.159999999999997</v>
+        <v>33.16</v>
       </c>
       <c r="K10" s="7">
-        <v>34.241999999999997</v>
+        <v>34.242</v>
       </c>
       <c r="L10" s="7">
         <v>32.31</v>
       </c>
       <c r="M10" s="7">
-        <v>32.780999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="4">
+        <v>32.781</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13">
+      <c r="B11" s="5">
         <v>7</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>6</v>
+      <c r="C11" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="D11" s="7">
         <v>42.4</v>
       </c>
       <c r="E11" s="7">
-        <v>42.489208504953837</v>
+        <v>42.4892085049538</v>
       </c>
       <c r="F11" s="7">
-        <v>41.384729999999998</v>
+        <v>41.38473</v>
       </c>
       <c r="G11" s="7">
         <v>44.3</v>
@@ -1021,30 +1616,30 @@
         <v>40.11</v>
       </c>
       <c r="K11" s="7">
-        <v>40.719000000000001</v>
+        <v>40.719</v>
       </c>
       <c r="L11" s="7">
         <v>39.56</v>
       </c>
       <c r="M11" s="7">
-        <v>39.287999999999997</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="4">
+        <v>39.288</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13">
+      <c r="B12" s="5">
         <v>8</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>7</v>
+      <c r="C12" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="D12" s="7">
         <v>66.2</v>
       </c>
       <c r="E12" s="7">
-        <v>66.339283090281683</v>
+        <v>66.3392830902817</v>
       </c>
       <c r="F12" s="7">
-        <v>64.558210000000003</v>
+        <v>64.55821</v>
       </c>
       <c r="G12" s="7">
         <v>63.9</v>
@@ -1059,30 +1654,30 @@
         <v>62.03</v>
       </c>
       <c r="K12" s="7">
-        <v>62.715000000000003</v>
+        <v>62.715</v>
       </c>
       <c r="L12" s="7">
         <v>60.08</v>
       </c>
       <c r="M12" s="7">
-        <v>58.896000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="4">
+        <v>58.896</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13">
+      <c r="B13" s="5">
         <v>9</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
+      <c r="C13" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="D13" s="7">
         <v>90.2</v>
       </c>
       <c r="E13" s="7">
-        <v>90.389778470444156</v>
+        <v>90.3897784704442</v>
       </c>
       <c r="F13" s="7">
-        <v>88.024870000000007</v>
+        <v>88.02487</v>
       </c>
       <c r="G13" s="7">
         <v>85.8</v>
@@ -1097,33 +1692,33 @@
         <v>90.16</v>
       </c>
       <c r="K13" s="7">
-        <v>92.344999999999999</v>
+        <v>92.345</v>
       </c>
       <c r="L13" s="7">
         <v>89.53</v>
       </c>
       <c r="M13" s="7">
-        <v>86.284999999999997</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="4">
+        <v>86.285</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13">
+      <c r="B14" s="5">
         <v>10</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>9</v>
+      <c r="C14" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="D14" s="7">
-        <v>76.099999999999994</v>
+        <v>76.1</v>
       </c>
       <c r="E14" s="7">
-        <v>76.260112434598668</v>
+        <v>76.2601124345987</v>
       </c>
       <c r="F14" s="7">
-        <v>74.296710000000004</v>
+        <v>74.29671</v>
       </c>
       <c r="G14" s="7">
-        <v>73.900000000000006</v>
+        <v>73.9</v>
       </c>
       <c r="H14" s="7">
         <v>72.2</v>
@@ -1135,27 +1730,27 @@
         <v>70.44</v>
       </c>
       <c r="K14" s="7">
-        <v>71.537999999999997</v>
+        <v>71.538</v>
       </c>
       <c r="L14" s="7">
-        <v>65.739999999999995</v>
+        <v>65.74</v>
       </c>
       <c r="M14" s="7">
-        <v>63.600999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="4">
+        <v>63.601</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13">
+      <c r="B15" s="5">
         <v>11</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>10</v>
+      <c r="C15" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="D15" s="7">
         <v>124.4</v>
       </c>
       <c r="E15" s="7">
-        <v>124.66173438717581</v>
+        <v>124.661734387176</v>
       </c>
       <c r="F15" s="7">
         <v>121.423</v>
@@ -1179,59 +1774,59 @@
         <v>111.27</v>
       </c>
       <c r="M15" s="7">
-        <v>107.34099999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="5">
+        <v>107.341</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13">
+      <c r="B16" s="8">
         <v>12</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="8">
+      <c r="C16" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="10">
         <v>25.2</v>
       </c>
-      <c r="E16" s="8">
-        <v>25.253020149170659</v>
-      </c>
-      <c r="F16" s="8">
-        <v>24.635449999999999</v>
-      </c>
-      <c r="G16" s="8">
+      <c r="E16" s="10">
+        <v>25.2530201491707</v>
+      </c>
+      <c r="F16" s="10">
+        <v>24.63545</v>
+      </c>
+      <c r="G16" s="10">
         <v>25.7</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="10">
         <v>25</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="10">
         <v>25.93</v>
       </c>
-      <c r="J16" s="8">
+      <c r="J16" s="10">
         <v>25.73</v>
       </c>
-      <c r="K16" s="8">
+      <c r="K16" s="10">
         <v>26.573</v>
       </c>
-      <c r="L16" s="8">
+      <c r="L16" s="10">
         <v>25.23</v>
       </c>
-      <c r="M16" s="8">
-        <v>24.364000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B17" s="4">
+      <c r="M16" s="10">
+        <v>24.364</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13">
+      <c r="B17" s="5">
         <v>13</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>12</v>
+      <c r="C17" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="D17" s="7">
         <v>19</v>
       </c>
       <c r="E17" s="7">
-        <v>19.140185906712677</v>
+        <v>19.1401859067127</v>
       </c>
       <c r="F17" s="7">
         <v>18.59806</v>
@@ -1240,7 +1835,7 @@
         <v>19</v>
       </c>
       <c r="H17" s="7">
-        <v>18.600000000000001</v>
+        <v>18.6</v>
       </c>
       <c r="I17" s="7">
         <v>19.32</v>
@@ -1258,33 +1853,33 @@
         <v>18.625</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B18" s="4">
+    <row r="18" spans="2:13">
+      <c r="B18" s="5">
         <v>14</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>13</v>
+      <c r="C18" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="D18" s="7">
         <v>45.2</v>
       </c>
       <c r="E18" s="7">
-        <v>45.295099632639435</v>
+        <v>45.2950996326394</v>
       </c>
       <c r="F18" s="7">
         <v>44.10933</v>
       </c>
       <c r="G18" s="7">
-        <v>40.799999999999997</v>
+        <v>40.8</v>
       </c>
       <c r="H18" s="7">
         <v>39.9</v>
       </c>
       <c r="I18" s="7">
-        <v>40.380000000000003</v>
+        <v>40.38</v>
       </c>
       <c r="J18" s="7">
-        <v>40.880000000000003</v>
+        <v>40.88</v>
       </c>
       <c r="K18" s="7">
         <v>42.012</v>
@@ -1293,27 +1888,27 @@
         <v>41.21</v>
       </c>
       <c r="M18" s="7">
-        <v>39.353000000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B19" s="4">
+        <v>39.353</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13">
+      <c r="B19" s="5">
         <v>15</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>14</v>
+      <c r="C19" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="D19" s="7">
         <v>33.4</v>
       </c>
       <c r="E19" s="7">
-        <v>33.570483134810182</v>
+        <v>33.5704831348102</v>
       </c>
       <c r="F19" s="7">
-        <v>32.718060000000001</v>
+        <v>32.71806</v>
       </c>
       <c r="G19" s="7">
-        <v>32.700000000000003</v>
+        <v>32.7</v>
       </c>
       <c r="H19" s="7">
         <v>31.9</v>
@@ -1325,27 +1920,27 @@
         <v>30.31</v>
       </c>
       <c r="K19" s="7">
-        <v>31.056999999999999</v>
+        <v>31.057</v>
       </c>
       <c r="L19" s="7">
         <v>31.06</v>
       </c>
       <c r="M19" s="7">
-        <v>29.931999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B20" s="4">
+        <v>29.932</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13">
+      <c r="B20" s="5">
         <v>16</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>15</v>
+      <c r="C20" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="D20" s="7">
         <v>15.6</v>
       </c>
       <c r="E20" s="7">
-        <v>15.632821997105653</v>
+        <v>15.6328219971057</v>
       </c>
       <c r="F20" s="7">
         <v>15.18998</v>
@@ -1372,21 +1967,21 @@
         <v>12.352</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B21" s="4">
+    <row r="21" spans="2:13">
+      <c r="B21" s="5">
         <v>17</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>16</v>
+      <c r="C21" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="D21" s="7">
         <v>32.1</v>
       </c>
       <c r="E21" s="7">
-        <v>32.167537570967347</v>
+        <v>32.1675375709673</v>
       </c>
       <c r="F21" s="7">
-        <v>31.353960000000001</v>
+        <v>31.35396</v>
       </c>
       <c r="G21" s="7">
         <v>30.9</v>
@@ -1401,30 +1996,30 @@
         <v>29.82</v>
       </c>
       <c r="K21" s="7">
-        <v>29.984999999999999</v>
+        <v>29.985</v>
       </c>
       <c r="L21" s="7">
         <v>29.08</v>
       </c>
       <c r="M21" s="7">
-        <v>28.451000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B22" s="4">
+        <v>28.451</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13">
+      <c r="B22" s="5">
         <v>18</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>17</v>
+      <c r="C22" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="D22" s="7">
-        <v>34.700000000000003</v>
+        <v>34.7</v>
       </c>
       <c r="E22" s="7">
-        <v>34.773007903818318</v>
+        <v>34.7730079038183</v>
       </c>
       <c r="F22" s="7">
-        <v>33.885660000000001</v>
+        <v>33.88566</v>
       </c>
       <c r="G22" s="7">
         <v>32.6</v>
@@ -1439,7 +2034,7 @@
         <v>31.94</v>
       </c>
       <c r="K22" s="7">
-        <v>33.598999999999997</v>
+        <v>33.599</v>
       </c>
       <c r="L22" s="7">
         <v>31.72</v>
@@ -1448,27 +2043,27 @@
         <v>30.974</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B23" s="4">
+    <row r="23" spans="2:13">
+      <c r="B23" s="5">
         <v>19</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>18</v>
+      <c r="C23" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="D23" s="7">
         <v>20.8</v>
       </c>
       <c r="E23" s="7">
-        <v>20.843762662807517</v>
+        <v>20.8437626628075</v>
       </c>
       <c r="F23" s="7">
         <v>20.25412</v>
       </c>
       <c r="G23" s="7">
-        <v>19.399999999999999</v>
+        <v>19.4</v>
       </c>
       <c r="H23" s="7">
-        <v>19.399999999999999</v>
+        <v>19.4</v>
       </c>
       <c r="I23" s="7">
         <v>19.3</v>
@@ -1477,27 +2072,27 @@
         <v>18.8</v>
       </c>
       <c r="K23" s="7">
-        <v>19.233000000000001</v>
+        <v>19.233</v>
       </c>
       <c r="L23" s="7">
         <v>19.13</v>
       </c>
       <c r="M23" s="7">
-        <v>19.420999999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B24" s="4">
+        <v>19.421</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13">
+      <c r="B24" s="5">
         <v>20</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>19</v>
+      <c r="C24" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="D24" s="7">
         <v>6.6</v>
       </c>
       <c r="E24" s="7">
-        <v>6.7140966269620392</v>
+        <v>6.71409662696204</v>
       </c>
       <c r="F24" s="7">
         <v>6.524127</v>
@@ -1521,24 +2116,24 @@
         <v>5.62</v>
       </c>
       <c r="M24" s="7">
-        <v>5.4279999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B25" s="4">
+        <v>5.428</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13">
+      <c r="B25" s="5">
         <v>21</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>20</v>
+      <c r="C25" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="D25" s="7">
         <v>22.4</v>
       </c>
       <c r="E25" s="7">
-        <v>22.447129021485019</v>
+        <v>22.447129021485</v>
       </c>
       <c r="F25" s="7">
-        <v>21.811119999999999</v>
+        <v>21.81112</v>
       </c>
       <c r="G25" s="7">
         <v>20.3</v>
@@ -1553,30 +2148,30 @@
         <v>18.63</v>
       </c>
       <c r="K25" s="7">
-        <v>19.204000000000001</v>
+        <v>19.204</v>
       </c>
       <c r="L25" s="7">
         <v>18.73</v>
       </c>
       <c r="M25" s="7">
-        <v>18.623999999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B26" s="4">
+        <v>18.624</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13">
+      <c r="B26" s="5">
         <v>22</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>21</v>
+      <c r="C26" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="D26" s="7">
         <v>24</v>
       </c>
       <c r="E26" s="7">
-        <v>24.150705777579876</v>
+        <v>24.1507057775799</v>
       </c>
       <c r="F26" s="7">
-        <v>23.563849999999999</v>
+        <v>23.56385</v>
       </c>
       <c r="G26" s="7">
         <v>23</v>
@@ -1591,27 +2186,27 @@
         <v>23.28</v>
       </c>
       <c r="K26" s="7">
-        <v>24.402999999999999</v>
+        <v>24.403</v>
       </c>
       <c r="L26" s="7">
         <v>23.88</v>
       </c>
       <c r="M26" s="7">
-        <v>23.050999999999998</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B27" s="4">
+        <v>23.051</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13">
+      <c r="B27" s="5">
         <v>23</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>22</v>
+      <c r="C27" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="D27" s="7">
-        <v>16.399999999999999</v>
+        <v>16.4</v>
       </c>
       <c r="E27" s="7">
-        <v>16.534715573861735</v>
+        <v>16.5347155738617</v>
       </c>
       <c r="F27" s="7">
         <v>16.06654</v>
@@ -1635,65 +2230,70 @@
         <v>14.78</v>
       </c>
       <c r="M27" s="7">
-        <v>14.563000000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="9">
-        <v>897.50000000000011</v>
-      </c>
-      <c r="E28" s="9">
+        <v>14.563</v>
+      </c>
+    </row>
+    <row r="28" ht="15" customHeight="1" spans="2:13">
+      <c r="B28" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="13">
+        <v>897.5</v>
+      </c>
+      <c r="E28" s="13">
         <v>900.19</v>
       </c>
-      <c r="F28" s="9">
-        <v>876.55341700000008</v>
-      </c>
-      <c r="G28" s="9">
+      <c r="F28" s="13">
+        <v>876.553417</v>
+      </c>
+      <c r="G28" s="13">
         <v>856.8</v>
       </c>
-      <c r="H28" s="9">
-        <v>837.30000000000007</v>
-      </c>
-      <c r="I28" s="9">
-        <v>851.57999999999981</v>
-      </c>
-      <c r="J28" s="9">
-        <v>848.43999999999994</v>
-      </c>
-      <c r="K28" s="9">
-        <v>872.61299999999994</v>
-      </c>
-      <c r="L28" s="9">
-        <v>839.49000000000012</v>
-      </c>
-      <c r="M28" s="9">
-        <v>819.44000000000017</v>
+      <c r="H28" s="13">
+        <v>837.3</v>
+      </c>
+      <c r="I28" s="13">
+        <v>851.58</v>
+      </c>
+      <c r="J28" s="13">
+        <v>848.44</v>
+      </c>
+      <c r="K28" s="13">
+        <v>872.613</v>
+      </c>
+      <c r="L28" s="13">
+        <v>839.49</v>
+      </c>
+      <c r="M28" s="13">
+        <v>819.44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="D3:M3"/>
     <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B1:M1"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>